<commit_message>
[modify] UMConfig Json 部分完成
</commit_message>
<xml_diff>
--- a/GameConfig/Bullet/bullet.xlsx
+++ b/GameConfig/Bullet/bullet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B469716-D504-4CB3-B444-D806E4A6A98E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE31951-2F26-4F35-8933-6CD5D8F8ED0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2172" yWindow="3396" windowWidth="20868" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -220,10 +220,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>s_max</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>9.856</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -334,6 +330,10 @@
   </si>
   <si>
     <t>875</t>
+  </si>
+  <si>
+    <t>s_Max</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -578,6 +578,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -589,39 +622,6 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -906,12 +906,12 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection sqref="A1:E1048576"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="15.77734375" style="17" customWidth="1"/>
+    <col min="1" max="5" width="15.77734375" style="13" customWidth="1"/>
     <col min="6" max="6" width="9" style="1"/>
     <col min="7" max="7" width="59.33203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="13.77734375" style="1" customWidth="1"/>
@@ -919,357 +919,357 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>70</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>51</v>
+      <c r="E2" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" s="15"/>
+    </row>
+    <row r="5" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E5" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="16" t="s">
+      <c r="G5" s="16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E6" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="16" t="s">
+      <c r="G6" s="17"/>
+    </row>
+    <row r="7" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" s="16" t="s">
+      <c r="E10" s="12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" s="16" t="s">
+      <c r="E13" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" s="16" t="s">
+      <c r="E14" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="16" t="s">
+      <c r="E15" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D11" s="16" t="s">
+      <c r="E18" s="12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D19" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D12" s="16" t="s">
+      <c r="E19" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="16" t="s">
+      <c r="E20" s="12" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="13.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="16" t="s">
-        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>